<commit_message>
Fixed typo in taxa name
</commit_message>
<xml_diff>
--- a/source_data/Swimming Speeds Raw Data.xlsx
+++ b/source_data/Swimming Speeds Raw Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aimsgovau-my.sharepoint.com/personal/r_fisher_aims_gov_au/Documents/Documents/AIMS/Ucrit_dataMS/source_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rworking_projects\tropical_ucrit_data\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{3D301261-9561-B542-A5B3-458647FEE670}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DC6204B2-A146-4BA1-A0F0-0B3F1A14D095}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81750A7D-D1A7-4B8B-90DB-858DDE7C83AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{28A6F4AC-483D-AB41-B7F8-6A8B88AF5E5C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28A6F4AC-483D-AB41-B7F8-6A8B88AF5E5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -813,9 +813,6 @@
     <t>Pempheridae</t>
   </si>
   <si>
-    <t>Gerridae</t>
-  </si>
-  <si>
     <t>Synodontidae</t>
   </si>
   <si>
@@ -889,6 +886,9 @@
   </si>
   <si>
     <t>Idiosepius pygmaeus</t>
+  </si>
+  <si>
+    <t>Gerreidae</t>
   </si>
 </sst>
 </file>
@@ -1651,57 +1651,72 @@
     <xf numFmtId="1" fontId="24" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1714,22 +1729,7 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -2048,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DC5F5D-F63C-6241-B044-EAC186D53D17}">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127:A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2100,11 +2100,11 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="83" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="8">
@@ -2123,11 +2123,11 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="82"/>
+      <c r="A4" s="78"/>
       <c r="B4" s="5">
         <v>47.5</v>
       </c>
@@ -2144,11 +2144,11 @@
         <v>65</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="82"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="5">
         <v>36.4</v>
       </c>
@@ -2165,11 +2165,11 @@
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="83"/>
+      <c r="A6" s="79"/>
       <c r="B6" s="5">
         <v>39.6</v>
       </c>
@@ -2183,14 +2183,14 @@
         <v>10</v>
       </c>
       <c r="F6" s="69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="84" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="5">
@@ -2207,11 +2207,11 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
+      <c r="A8" s="85"/>
       <c r="B8" s="5">
         <v>35.200000000000003</v>
       </c>
@@ -2228,11 +2228,11 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
+      <c r="A9" s="85"/>
       <c r="B9" s="5">
         <v>38.799999999999997</v>
       </c>
@@ -2249,11 +2249,11 @@
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
+      <c r="A10" s="85"/>
       <c r="B10" s="5">
         <v>38.9</v>
       </c>
@@ -2270,11 +2270,11 @@
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="100"/>
+      <c r="A11" s="86"/>
       <c r="B11" s="4">
         <v>39</v>
       </c>
@@ -2291,12 +2291,12 @@
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="97" t="s">
-        <v>73</v>
+      <c r="A12" s="83" t="s">
+        <v>72</v>
       </c>
       <c r="B12" s="5">
         <v>32.6</v>
@@ -2314,11 +2314,11 @@
         <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="99"/>
+      <c r="A13" s="85"/>
       <c r="B13" s="5">
         <v>36.5</v>
       </c>
@@ -2335,11 +2335,11 @@
         <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="100"/>
+      <c r="A14" s="86"/>
       <c r="B14" s="5">
         <v>32.4</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.25">
@@ -2376,10 +2376,10 @@
         <v>17</v>
       </c>
       <c r="F15" s="69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="77" t="s">
         <v>62</v>
       </c>
       <c r="B17" s="16">
@@ -2429,7 +2429,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="16">
         <v>13.4</v>
       </c>
@@ -2450,7 +2450,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="74" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="16">
@@ -2469,11 +2469,11 @@
         <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="79"/>
+      <c r="A20" s="75"/>
       <c r="B20" s="16">
         <v>36.299999999999997</v>
       </c>
@@ -2490,11 +2490,11 @@
         <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
+      <c r="A21" s="76"/>
       <c r="B21" s="16">
         <v>15.5</v>
       </c>
@@ -2511,11 +2511,11 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="74" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="16">
@@ -2534,11 +2534,11 @@
         <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="79"/>
+      <c r="A23" s="75"/>
       <c r="B23" s="16">
         <v>20.6</v>
       </c>
@@ -2555,11 +2555,11 @@
         <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="79"/>
+      <c r="A24" s="75"/>
       <c r="B24" s="16">
         <v>18.899999999999999</v>
       </c>
@@ -2576,11 +2576,11 @@
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="75"/>
+      <c r="A25" s="76"/>
       <c r="B25" s="16">
         <v>18.899999999999999</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="33" x14ac:dyDescent="0.25">
@@ -2620,12 +2620,12 @@
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="95" t="s">
-        <v>70</v>
+      <c r="A27" s="77" t="s">
+        <v>69</v>
       </c>
       <c r="B27" s="23">
         <v>21.6</v>
@@ -2643,11 +2643,11 @@
         <v>28</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="82"/>
+      <c r="A28" s="78"/>
       <c r="B28" s="23">
         <v>9.1999999999999993</v>
       </c>
@@ -2668,7 +2668,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="82"/>
+      <c r="A29" s="78"/>
       <c r="B29" s="23">
         <v>9.6</v>
       </c>
@@ -2689,7 +2689,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="82"/>
+      <c r="A30" s="78"/>
       <c r="B30" s="23">
         <v>9.6</v>
       </c>
@@ -2710,7 +2710,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="82"/>
+      <c r="A31" s="78"/>
       <c r="B31" s="23">
         <v>9.6999999999999993</v>
       </c>
@@ -2731,7 +2731,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
+      <c r="A32" s="79"/>
       <c r="B32" s="23">
         <v>9.6999999999999993</v>
       </c>
@@ -2752,8 +2752,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="96" t="s">
-        <v>74</v>
+      <c r="A33" s="80" t="s">
+        <v>73</v>
       </c>
       <c r="B33" s="23">
         <v>26.8</v>
@@ -2771,11 +2771,11 @@
         <v>50</v>
       </c>
       <c r="G33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="85"/>
+      <c r="A34" s="81"/>
       <c r="B34" s="23">
         <v>27.1</v>
       </c>
@@ -2792,11 +2792,11 @@
         <v>65</v>
       </c>
       <c r="G34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="85"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="23">
         <v>29.7</v>
       </c>
@@ -2813,11 +2813,11 @@
         <v>65</v>
       </c>
       <c r="G35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="85"/>
+      <c r="A36" s="81"/>
       <c r="B36" s="23">
         <v>25.7</v>
       </c>
@@ -2834,11 +2834,11 @@
         <v>60</v>
       </c>
       <c r="G36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="85"/>
+      <c r="A37" s="81"/>
       <c r="B37" s="23">
         <v>32.299999999999997</v>
       </c>
@@ -2855,11 +2855,11 @@
         <v>60</v>
       </c>
       <c r="G37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="85"/>
+      <c r="A38" s="81"/>
       <c r="B38" s="21">
         <v>34</v>
       </c>
@@ -2876,11 +2876,11 @@
         <v>29</v>
       </c>
       <c r="G38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="85"/>
+      <c r="A39" s="81"/>
       <c r="B39" s="23">
         <v>29.4</v>
       </c>
@@ -2897,11 +2897,11 @@
         <v>70</v>
       </c>
       <c r="G39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="85"/>
+      <c r="A40" s="81"/>
       <c r="B40" s="23">
         <v>26.5</v>
       </c>
@@ -2918,11 +2918,11 @@
         <v>70</v>
       </c>
       <c r="G40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="85"/>
+      <c r="A41" s="81"/>
       <c r="B41" s="23">
         <v>22.3</v>
       </c>
@@ -2939,11 +2939,11 @@
         <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="85"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="21">
         <v>29</v>
       </c>
@@ -2960,11 +2960,11 @@
         <v>70</v>
       </c>
       <c r="G42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="85"/>
+      <c r="A43" s="81"/>
       <c r="B43" s="23">
         <v>32.1</v>
       </c>
@@ -2981,11 +2981,11 @@
         <v>29</v>
       </c>
       <c r="G43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="85"/>
+      <c r="A44" s="81"/>
       <c r="B44" s="23">
         <v>30.9</v>
       </c>
@@ -3002,11 +3002,11 @@
         <v>65</v>
       </c>
       <c r="G44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="85"/>
+      <c r="A45" s="81"/>
       <c r="B45" s="71">
         <v>32.6</v>
       </c>
@@ -3023,11 +3023,11 @@
         <v>60</v>
       </c>
       <c r="G45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="85"/>
+      <c r="A46" s="81"/>
       <c r="B46" s="21">
         <v>23</v>
       </c>
@@ -3044,11 +3044,11 @@
         <v>60</v>
       </c>
       <c r="G46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="85"/>
+      <c r="A47" s="81"/>
       <c r="B47" s="23">
         <v>22.7</v>
       </c>
@@ -3065,11 +3065,11 @@
         <v>65</v>
       </c>
       <c r="G47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="85"/>
+      <c r="A48" s="81"/>
       <c r="B48" s="23">
         <v>37.799999999999997</v>
       </c>
@@ -3086,11 +3086,11 @@
         <v>70</v>
       </c>
       <c r="G48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="85"/>
+      <c r="A49" s="81"/>
       <c r="B49" s="23">
         <v>38.700000000000003</v>
       </c>
@@ -3107,11 +3107,11 @@
         <v>70</v>
       </c>
       <c r="G49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="85"/>
+      <c r="A50" s="81"/>
       <c r="B50" s="23">
         <v>26.2</v>
       </c>
@@ -3128,11 +3128,11 @@
         <v>29</v>
       </c>
       <c r="G50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="85"/>
+      <c r="A51" s="81"/>
       <c r="B51" s="21">
         <v>28</v>
       </c>
@@ -3149,11 +3149,11 @@
         <v>29</v>
       </c>
       <c r="G51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="85"/>
+      <c r="A52" s="81"/>
       <c r="B52" s="34">
         <v>27.4</v>
       </c>
@@ -3170,11 +3170,11 @@
         <v>65</v>
       </c>
       <c r="G52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="85"/>
+      <c r="A53" s="81"/>
       <c r="B53" s="34">
         <v>24.3</v>
       </c>
@@ -3191,11 +3191,11 @@
         <v>29</v>
       </c>
       <c r="G53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="85"/>
+      <c r="A54" s="81"/>
       <c r="B54" s="34">
         <v>29.2</v>
       </c>
@@ -3212,11 +3212,11 @@
         <v>70</v>
       </c>
       <c r="G54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="85"/>
+      <c r="A55" s="81"/>
       <c r="B55" s="36">
         <v>28</v>
       </c>
@@ -3233,11 +3233,11 @@
         <v>70</v>
       </c>
       <c r="G55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="85"/>
+      <c r="A56" s="81"/>
       <c r="B56" s="34">
         <v>32.700000000000003</v>
       </c>
@@ -3254,11 +3254,11 @@
         <v>65</v>
       </c>
       <c r="G56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="86"/>
+      <c r="A57" s="82"/>
       <c r="B57" s="36">
         <v>28</v>
       </c>
@@ -3275,12 +3275,12 @@
         <v>29</v>
       </c>
       <c r="G57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="81" t="s">
-        <v>69</v>
+      <c r="A58" s="89" t="s">
+        <v>68</v>
       </c>
       <c r="B58" s="5">
         <v>51.8</v>
@@ -3298,11 +3298,11 @@
         <v>32</v>
       </c>
       <c r="G58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="79"/>
+      <c r="A59" s="75"/>
       <c r="B59" s="5">
         <v>62.7</v>
       </c>
@@ -3319,11 +3319,11 @@
         <v>32</v>
       </c>
       <c r="G59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="79"/>
+      <c r="A60" s="75"/>
       <c r="B60" s="5">
         <v>43.5</v>
       </c>
@@ -3340,11 +3340,11 @@
         <v>32</v>
       </c>
       <c r="G60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="75"/>
+      <c r="A61" s="76"/>
       <c r="B61" s="5">
         <v>55.7</v>
       </c>
@@ -3361,11 +3361,11 @@
         <v>32</v>
       </c>
       <c r="G61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="80" t="s">
+      <c r="A62" s="74" t="s">
         <v>33</v>
       </c>
       <c r="B62" s="5">
@@ -3384,11 +3384,11 @@
         <v>30</v>
       </c>
       <c r="G62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="79"/>
+      <c r="A63" s="75"/>
       <c r="B63" s="5">
         <v>48.1</v>
       </c>
@@ -3405,11 +3405,11 @@
         <v>45</v>
       </c>
       <c r="G63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="79"/>
+      <c r="A64" s="75"/>
       <c r="B64" s="4">
         <v>53</v>
       </c>
@@ -3426,11 +3426,11 @@
         <v>60</v>
       </c>
       <c r="G64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="79"/>
+      <c r="A65" s="75"/>
       <c r="B65" s="5">
         <v>50.2</v>
       </c>
@@ -3447,11 +3447,11 @@
         <v>35</v>
       </c>
       <c r="G65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="75"/>
+      <c r="A66" s="76"/>
       <c r="B66" s="5">
         <v>27.5</v>
       </c>
@@ -3468,12 +3468,12 @@
         <v>32</v>
       </c>
       <c r="G66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="81" t="s">
-        <v>78</v>
+      <c r="A67" s="89" t="s">
+        <v>77</v>
       </c>
       <c r="B67" s="5">
         <v>33.5</v>
@@ -3491,11 +3491,11 @@
         <v>50</v>
       </c>
       <c r="G67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A68" s="79"/>
+      <c r="A68" s="75"/>
       <c r="B68" s="5">
         <v>39.700000000000003</v>
       </c>
@@ -3512,11 +3512,11 @@
         <v>55</v>
       </c>
       <c r="G68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="75"/>
+      <c r="A69" s="76"/>
       <c r="B69" s="5">
         <v>53.6</v>
       </c>
@@ -3533,12 +3533,12 @@
         <v>32</v>
       </c>
       <c r="G69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="81" t="s">
-        <v>71</v>
+      <c r="A70" s="89" t="s">
+        <v>70</v>
       </c>
       <c r="B70" s="5">
         <v>42.8</v>
@@ -3556,11 +3556,11 @@
         <v>35</v>
       </c>
       <c r="G70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="82"/>
+      <c r="A71" s="78"/>
       <c r="B71" s="5">
         <v>43.4</v>
       </c>
@@ -3577,11 +3577,11 @@
         <v>30</v>
       </c>
       <c r="G71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="82"/>
+      <c r="A72" s="78"/>
       <c r="B72" s="5">
         <v>61.5</v>
       </c>
@@ -3598,11 +3598,11 @@
         <v>55</v>
       </c>
       <c r="G72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="82"/>
+      <c r="A73" s="78"/>
       <c r="B73" s="40">
         <v>39.799999999999997</v>
       </c>
@@ -3619,11 +3619,11 @@
         <v>65</v>
       </c>
       <c r="G73" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="82"/>
+      <c r="A74" s="78"/>
       <c r="B74" s="5">
         <v>25.1</v>
       </c>
@@ -3640,11 +3640,11 @@
         <v>20</v>
       </c>
       <c r="G74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="82"/>
+      <c r="A75" s="78"/>
       <c r="B75" s="42">
         <v>53</v>
       </c>
@@ -3661,11 +3661,11 @@
         <v>35</v>
       </c>
       <c r="G75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="82"/>
+      <c r="A76" s="78"/>
       <c r="B76" s="5">
         <v>40.1</v>
       </c>
@@ -3682,11 +3682,11 @@
         <v>32</v>
       </c>
       <c r="G76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="82"/>
+      <c r="A77" s="78"/>
       <c r="B77" s="40">
         <v>32.1</v>
       </c>
@@ -3703,11 +3703,11 @@
         <v>35</v>
       </c>
       <c r="G77" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="83"/>
+      <c r="A78" s="79"/>
       <c r="B78" s="40">
         <v>39.5</v>
       </c>
@@ -3724,12 +3724,12 @@
         <v>45</v>
       </c>
       <c r="G78" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="84" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A79" s="90" t="s">
+        <v>78</v>
       </c>
       <c r="B79" s="5">
         <v>42.2</v>
@@ -3747,11 +3747,11 @@
         <v>35</v>
       </c>
       <c r="G79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="85"/>
+      <c r="A80" s="81"/>
       <c r="B80" s="5">
         <v>42.6</v>
       </c>
@@ -3768,11 +3768,11 @@
         <v>30</v>
       </c>
       <c r="G80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="85"/>
+      <c r="A81" s="81"/>
       <c r="B81" s="40">
         <v>37.9</v>
       </c>
@@ -3789,11 +3789,11 @@
         <v>40</v>
       </c>
       <c r="G81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="85"/>
+      <c r="A82" s="81"/>
       <c r="B82" s="40">
         <v>38.6</v>
       </c>
@@ -3810,11 +3810,11 @@
         <v>65</v>
       </c>
       <c r="G82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="85"/>
+      <c r="A83" s="81"/>
       <c r="B83" s="40">
         <v>31.1</v>
       </c>
@@ -3831,11 +3831,11 @@
         <v>20</v>
       </c>
       <c r="G83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="85"/>
+      <c r="A84" s="81"/>
       <c r="B84" s="40">
         <v>41.4</v>
       </c>
@@ -3852,11 +3852,11 @@
         <v>40</v>
       </c>
       <c r="G84" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="86"/>
+      <c r="A85" s="82"/>
       <c r="B85" s="42">
         <v>40</v>
       </c>
@@ -3873,11 +3873,11 @@
         <v>30</v>
       </c>
       <c r="G85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="87" t="s">
+      <c r="A86" s="91" t="s">
         <v>36</v>
       </c>
       <c r="B86" s="40">
@@ -3896,11 +3896,11 @@
         <v>30</v>
       </c>
       <c r="G86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="88"/>
+      <c r="A87" s="92"/>
       <c r="B87" s="40">
         <v>26.3</v>
       </c>
@@ -3917,11 +3917,11 @@
         <v>35</v>
       </c>
       <c r="G87" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="88"/>
+      <c r="A88" s="92"/>
       <c r="B88" s="40">
         <v>28.7</v>
       </c>
@@ -3938,11 +3938,11 @@
         <v>50</v>
       </c>
       <c r="G88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="88"/>
+      <c r="A89" s="92"/>
       <c r="B89" s="46">
         <v>28.4</v>
       </c>
@@ -3959,11 +3959,11 @@
         <v>35</v>
       </c>
       <c r="G89" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="88"/>
+      <c r="A90" s="92"/>
       <c r="B90" s="46">
         <v>30.6</v>
       </c>
@@ -3980,11 +3980,11 @@
         <v>60</v>
       </c>
       <c r="G90" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="88"/>
+      <c r="A91" s="92"/>
       <c r="B91" s="46">
         <v>30.8</v>
       </c>
@@ -4001,11 +4001,11 @@
         <v>50</v>
       </c>
       <c r="G91" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="88"/>
+      <c r="A92" s="92"/>
       <c r="B92" s="46">
         <v>34.4</v>
       </c>
@@ -4022,11 +4022,11 @@
         <v>45</v>
       </c>
       <c r="G92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="88"/>
+      <c r="A93" s="92"/>
       <c r="B93" s="46">
         <v>37.1</v>
       </c>
@@ -4043,11 +4043,11 @@
         <v>38</v>
       </c>
       <c r="G93" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="88"/>
+      <c r="A94" s="92"/>
       <c r="B94" s="46">
         <v>40.1</v>
       </c>
@@ -4064,11 +4064,11 @@
         <v>50</v>
       </c>
       <c r="G94" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="88"/>
+      <c r="A95" s="92"/>
       <c r="B95" s="49">
         <v>35</v>
       </c>
@@ -4085,11 +4085,11 @@
         <v>38</v>
       </c>
       <c r="G95" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="88"/>
+      <c r="A96" s="92"/>
       <c r="B96" s="46">
         <v>36.700000000000003</v>
       </c>
@@ -4106,11 +4106,11 @@
         <v>38</v>
       </c>
       <c r="G96" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="88"/>
+      <c r="A97" s="92"/>
       <c r="B97" s="46">
         <v>28.9</v>
       </c>
@@ -4127,11 +4127,11 @@
         <v>60</v>
       </c>
       <c r="G97" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="89"/>
+      <c r="A98" s="93"/>
       <c r="B98" s="46">
         <v>28.8</v>
       </c>
@@ -4146,12 +4146,12 @@
       </c>
       <c r="F98" s="52"/>
       <c r="G98" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="80" t="s">
-        <v>80</v>
+      <c r="A99" s="74" t="s">
+        <v>79</v>
       </c>
       <c r="B99" s="46">
         <v>11.9</v>
@@ -4169,11 +4169,11 @@
         <v>41</v>
       </c>
       <c r="G99" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="75"/>
+      <c r="A100" s="76"/>
       <c r="B100" s="46">
         <v>29.8</v>
       </c>
@@ -4190,12 +4190,12 @@
         <v>43</v>
       </c>
       <c r="G100" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A101" s="90" t="s">
-        <v>77</v>
+      <c r="A101" s="94" t="s">
+        <v>76</v>
       </c>
       <c r="B101" s="46">
         <v>24.9</v>
@@ -4213,11 +4213,11 @@
         <v>20</v>
       </c>
       <c r="G101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="78"/>
+      <c r="A102" s="95"/>
       <c r="B102" s="53">
         <v>9.4</v>
       </c>
@@ -4234,11 +4234,11 @@
         <v>26</v>
       </c>
       <c r="G102" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="78"/>
+      <c r="A103" s="95"/>
       <c r="B103" s="46">
         <v>24.1</v>
       </c>
@@ -4255,11 +4255,11 @@
         <v>50</v>
       </c>
       <c r="G103" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="77"/>
+      <c r="A104" s="88"/>
       <c r="B104" s="48">
         <v>13.25</v>
       </c>
@@ -4276,11 +4276,11 @@
         <v>10</v>
       </c>
       <c r="G104" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A105" s="91" t="s">
+      <c r="A105" s="96" t="s">
         <v>63</v>
       </c>
       <c r="B105" s="53">
@@ -4299,11 +4299,11 @@
         <v>10</v>
       </c>
       <c r="G105" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A106" s="92"/>
+      <c r="A106" s="97"/>
       <c r="B106" s="46">
         <v>35.5</v>
       </c>
@@ -4320,11 +4320,11 @@
         <v>11</v>
       </c>
       <c r="G106" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="93"/>
+      <c r="A107" s="98"/>
       <c r="B107" s="49">
         <v>11</v>
       </c>
@@ -4341,12 +4341,12 @@
         <v>16</v>
       </c>
       <c r="G107" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="90" t="s">
-        <v>77</v>
+      <c r="A108" s="94" t="s">
+        <v>76</v>
       </c>
       <c r="B108" s="46">
         <v>37.799999999999997</v>
@@ -4364,11 +4364,11 @@
         <v>60</v>
       </c>
       <c r="G108" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="78"/>
+      <c r="A109" s="95"/>
       <c r="B109" s="46">
         <v>42.9</v>
       </c>
@@ -4385,11 +4385,11 @@
         <v>66</v>
       </c>
       <c r="G109" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A110" s="77"/>
+      <c r="A110" s="88"/>
       <c r="B110" s="46">
         <v>41.1</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>40</v>
       </c>
       <c r="G110" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4429,12 +4429,12 @@
         <v>22</v>
       </c>
       <c r="G111" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A112" s="94" t="s">
-        <v>75</v>
+      <c r="A112" s="99" t="s">
+        <v>74</v>
       </c>
       <c r="B112" s="53">
         <v>35.5</v>
@@ -4452,11 +4452,11 @@
         <v>50</v>
       </c>
       <c r="G112" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A113" s="79"/>
+      <c r="A113" s="75"/>
       <c r="B113" s="53">
         <v>36.5</v>
       </c>
@@ -4473,11 +4473,11 @@
         <v>45</v>
       </c>
       <c r="G113" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="79"/>
+      <c r="A114" s="75"/>
       <c r="B114" s="53">
         <v>28.5</v>
       </c>
@@ -4494,11 +4494,11 @@
         <v>48</v>
       </c>
       <c r="G114" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A115" s="75"/>
+      <c r="A115" s="76"/>
       <c r="B115" s="53">
         <v>27.3</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>48</v>
       </c>
       <c r="G115" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -4538,12 +4538,12 @@
         <v>15</v>
       </c>
       <c r="G116" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A117" s="70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B117" s="53">
         <v>21.8</v>
@@ -4561,12 +4561,12 @@
         <v>45</v>
       </c>
       <c r="G117" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="76" t="s">
-        <v>76</v>
+      <c r="A118" s="87" t="s">
+        <v>75</v>
       </c>
       <c r="B118" s="57">
         <v>15</v>
@@ -4584,11 +4584,11 @@
         <v>45</v>
       </c>
       <c r="G118" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="78"/>
+      <c r="A119" s="95"/>
       <c r="B119" s="57">
         <v>15</v>
       </c>
@@ -4605,11 +4605,11 @@
         <v>65</v>
       </c>
       <c r="G119" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A120" s="77"/>
+      <c r="A120" s="88"/>
       <c r="B120" s="58">
         <v>15.7</v>
       </c>
@@ -4626,12 +4626,12 @@
         <v>60</v>
       </c>
       <c r="G120" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A121" s="76" t="s">
-        <v>68</v>
+      <c r="A121" s="87" t="s">
+        <v>67</v>
       </c>
       <c r="B121" s="57">
         <v>9</v>
@@ -4653,7 +4653,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A122" s="77"/>
+      <c r="A122" s="88"/>
       <c r="B122" s="58">
         <v>8.6</v>
       </c>
@@ -4674,7 +4674,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A123" s="74" t="s">
+      <c r="A123" s="100" t="s">
         <v>64</v>
       </c>
       <c r="B123" s="58">
@@ -4693,11 +4693,11 @@
         <v>46</v>
       </c>
       <c r="G123" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="75"/>
+      <c r="A124" s="76"/>
       <c r="B124" s="58">
         <v>20.399999999999999</v>
       </c>
@@ -4714,11 +4714,11 @@
         <v>10</v>
       </c>
       <c r="G124" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="76" t="s">
+      <c r="A125" s="87" t="s">
         <v>65</v>
       </c>
       <c r="B125" s="58">
@@ -4735,11 +4735,11 @@
       </c>
       <c r="F125" s="52"/>
       <c r="G125" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="77"/>
+      <c r="A126" s="88"/>
       <c r="B126" s="58">
         <v>8.4</v>
       </c>
@@ -4756,12 +4756,12 @@
         <v>6</v>
       </c>
       <c r="G126" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="76" t="s">
-        <v>66</v>
+      <c r="A127" s="87" t="s">
+        <v>85</v>
       </c>
       <c r="B127" s="58">
         <v>9.6999999999999993</v>
@@ -4779,11 +4779,11 @@
         <v>25</v>
       </c>
       <c r="G127" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A128" s="78"/>
+      <c r="A128" s="95"/>
       <c r="B128" s="58">
         <v>11.3</v>
       </c>
@@ -4800,11 +4800,11 @@
         <v>20</v>
       </c>
       <c r="G128" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="78"/>
+      <c r="A129" s="95"/>
       <c r="B129" s="58">
         <v>11.5</v>
       </c>
@@ -4821,11 +4821,11 @@
         <v>24</v>
       </c>
       <c r="G129" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A130" s="77"/>
+      <c r="A130" s="88"/>
       <c r="B130" s="58">
         <v>12.4</v>
       </c>
@@ -4842,12 +4842,12 @@
         <v>34</v>
       </c>
       <c r="G130" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A131" s="68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B131" s="58">
         <v>48.8</v>
@@ -4865,12 +4865,12 @@
         <v>40</v>
       </c>
       <c r="G131" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A132" s="68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B132" s="58">
         <v>27.6</v>
@@ -4888,12 +4888,12 @@
         <v>50</v>
       </c>
       <c r="G132" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A133" s="100" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A133" s="74" t="s">
-        <v>85</v>
       </c>
       <c r="B133" s="57">
         <v>8</v>
@@ -4911,11 +4911,11 @@
         <v>20</v>
       </c>
       <c r="G133" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="75"/>
+      <c r="A134" s="76"/>
       <c r="B134" s="57">
         <v>15</v>
       </c>
@@ -4932,12 +4932,12 @@
         <v>45</v>
       </c>
       <c r="G134" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="74" t="s">
-        <v>83</v>
+      <c r="A135" s="100" t="s">
+        <v>82</v>
       </c>
       <c r="B135" s="63">
         <v>8.9</v>
@@ -4955,11 +4955,11 @@
         <v>5</v>
       </c>
       <c r="G135" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="79"/>
+      <c r="A136" s="75"/>
       <c r="B136" s="63">
         <v>9.6999999999999993</v>
       </c>
@@ -4976,11 +4976,11 @@
         <v>5</v>
       </c>
       <c r="G136" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A137" s="79"/>
+      <c r="A137" s="75"/>
       <c r="B137" s="58">
         <v>6.5</v>
       </c>
@@ -4997,11 +4997,11 @@
         <v>5</v>
       </c>
       <c r="G137" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="79"/>
+      <c r="A138" s="75"/>
       <c r="B138" s="58">
         <v>14.5</v>
       </c>
@@ -5018,11 +5018,11 @@
         <v>5</v>
       </c>
       <c r="G138" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A139" s="79"/>
+      <c r="A139" s="75"/>
       <c r="B139" s="57">
         <v>13</v>
       </c>
@@ -5039,11 +5039,11 @@
         <v>5</v>
       </c>
       <c r="G139" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A140" s="79"/>
+      <c r="A140" s="75"/>
       <c r="B140" s="60">
         <v>11</v>
       </c>
@@ -5060,11 +5060,11 @@
         <v>5</v>
       </c>
       <c r="G140" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A141" s="79"/>
+      <c r="A141" s="75"/>
       <c r="B141" s="57">
         <v>13</v>
       </c>
@@ -5081,11 +5081,11 @@
         <v>5</v>
       </c>
       <c r="G141" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A142" s="79"/>
+      <c r="A142" s="75"/>
       <c r="B142" s="58">
         <v>13.5</v>
       </c>
@@ -5102,11 +5102,11 @@
         <v>5</v>
       </c>
       <c r="G142" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A143" s="79"/>
+      <c r="A143" s="75"/>
       <c r="B143" s="65">
         <v>12</v>
       </c>
@@ -5123,11 +5123,11 @@
         <v>5</v>
       </c>
       <c r="G143" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A144" s="79"/>
+      <c r="A144" s="75"/>
       <c r="B144" s="65">
         <v>7</v>
       </c>
@@ -5144,11 +5144,11 @@
         <v>5</v>
       </c>
       <c r="G144" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A145" s="75"/>
+      <c r="A145" s="76"/>
       <c r="B145" s="65">
         <v>9</v>
       </c>
@@ -5165,19 +5165,17 @@
         <v>20</v>
       </c>
       <c r="G145" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="A33:A57"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A135:A145"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="A127:A130"/>
+    <mergeCell ref="A133:A134"/>
     <mergeCell ref="A121:A122"/>
     <mergeCell ref="A62:A66"/>
     <mergeCell ref="A67:A69"/>
@@ -5190,12 +5188,14 @@
     <mergeCell ref="A108:A110"/>
     <mergeCell ref="A112:A115"/>
     <mergeCell ref="A118:A120"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="A127:A130"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="A135:A145"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A33:A57"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>